<commit_message>
inventar einlesen, waffe / rüstung ausrüsten, trefferprobe
</commit_message>
<xml_diff>
--- a/data/dsa5_talente.xlsx
+++ b/data/dsa5_talente.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SRH\Documents\GitHub\srh_proj_dsa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEA8DEB-9EA6-4841-A3EB-A0E7E559DC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7419B192-B874-4158-934A-4341C9BEC26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -386,10 +386,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">

</xml_diff>